<commit_message>
Corrected Dutch name of Assigning Authority
</commit_message>
<xml_diff>
--- a/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-rc.1.xlsx
+++ b/dataset/Dataset_MedMij_Beeldbeschikbaarheid_1.0.0-rc.1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4246830-322D-214E-9896-317A13BED8CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C1F00B3-20E5-2C43-8660-5892D8B8CA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="660" windowWidth="38080" windowHeight="19380" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
+    <workbookView xWindow="140" yWindow="540" windowWidth="38080" windowHeight="19380" activeTab="1" xr2:uid="{B1E2DBBA-4EE0-4C1E-8D8A-42B6775C8263}"/>
   </bookViews>
   <sheets>
     <sheet name="Beeld en verslag tijdlijn raadp" sheetId="3" r:id="rId1"/>
@@ -713,9 +713,6 @@
     <t>Het medische beeldvormingsapparaat, zoals een CT-scanner of een MRI-machine, dat wordt gebruikt om de beelden te verkrijgen.</t>
   </si>
   <si>
-    <t>2.4.1 AccessionNumber</t>
-  </si>
-  <si>
     <t>2.4. AccessionNumberInformatie</t>
   </si>
   <si>
@@ -768,9 +765,6 @@
   </si>
   <si>
     <t>2.1.5. Locatie</t>
-  </si>
-  <si>
-    <t>2.4.2 UitgevendeInstantie</t>
   </si>
   <si>
     <t>Uitgevende instantie van het Accession Number.</t>
@@ -838,13 +832,19 @@
   </si>
   <si>
     <t>  2.1.6.1.4. ZorgverlenerRol</t>
+  </si>
+  <si>
+    <t>2.4.1. AccessionNumber</t>
+  </si>
+  <si>
+    <t>2.4.2. UitgevendeInstantie</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="21">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1398,10 +1398,10 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="25" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30" customBuiltin="1"/>
@@ -1762,7 +1762,7 @@
       <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="17.5" customWidth="1"/>
     <col min="2" max="5" width="11" customWidth="1"/>
@@ -1770,7 +1770,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="2" customHeight="1">
       <c r="A2" s="66" t="s">
         <v>12</v>
       </c>
@@ -1821,7 +1821,7 @@
       <c r="D2" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="70" t="s">
+      <c r="E2" s="68" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="66" t="s">
@@ -1830,39 +1830,34 @@
       <c r="G2" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="68"/>
-      <c r="I2" s="68"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
       <c r="J2" s="66" t="s">
         <v>19</v>
       </c>
       <c r="K2" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="70" t="s">
+      <c r="L2" s="68" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1">
       <c r="A3" s="67"/>
       <c r="B3" s="67"/>
       <c r="C3" s="67"/>
       <c r="D3" s="67"/>
-      <c r="E3" s="71"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
       <c r="J3" s="67"/>
       <c r="K3" s="67"/>
-      <c r="L3" s="71"/>
+      <c r="L3" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="G2:G3"/>
@@ -1870,6 +1865,11 @@
     <mergeCell ref="L2:L3"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="J2:J3"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="E2:E3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="L2" r:id="rId1" display="http://decor.nictiz.nl/decor/services/RetrieveDataSet?conceptId=2.16.840.1.113883.2.4.3.11.60.40.1.0.1.7&amp;conceptEffectiveDate=2020-09-01T00:00:00&amp;format=html&amp;language=nl-NL&amp;seetype=live-services" xr:uid="{3CDAD70A-3BBE-4CDA-810F-FA2B5C6B897A}"/>
@@ -1884,10 +1884,10 @@
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="26.5" style="55" customWidth="1"/>
     <col min="2" max="2" width="21.83203125" style="37" customWidth="1"/>
@@ -1902,7 +1902,7 @@
     <col min="242" max="16384" width="8.83203125" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" s="10" customFormat="1">
       <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
@@ -1940,7 +1940,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" s="34" customFormat="1">
       <c r="A2" s="40" t="s">
         <v>22</v>
       </c>
@@ -1964,7 +1964,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" s="10" customFormat="1">
       <c r="A3" s="41" t="s">
         <v>27</v>
       </c>
@@ -1991,7 +1991,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" s="10" customFormat="1">
       <c r="A4" s="42" t="s">
         <v>31</v>
       </c>
@@ -2023,12 +2023,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" s="10" customFormat="1">
       <c r="A5" s="53" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C5" s="32" t="s">
         <v>14</v>
@@ -2040,7 +2040,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G5" s="34"/>
       <c r="H5" s="34"/>
@@ -2052,12 +2052,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="33" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" s="10" customFormat="1">
       <c r="A6" s="43" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>38</v>
@@ -2085,9 +2085,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" s="10" customFormat="1">
       <c r="A7" s="42" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>41</v>
@@ -2117,9 +2117,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" s="10" customFormat="1">
       <c r="A8" s="42" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>45</v>
@@ -2149,7 +2149,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" s="10" customFormat="1" ht="17.25" customHeight="1">
       <c r="A9" s="44" t="s">
         <v>48</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" s="10" customFormat="1" ht="18.75" customHeight="1">
       <c r="A10" s="45" t="s">
         <v>50</v>
       </c>
@@ -2213,7 +2213,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" s="10" customFormat="1">
       <c r="A11" s="45" t="s">
         <v>56</v>
       </c>
@@ -2247,7 +2247,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" s="10" customFormat="1">
       <c r="A12" s="46" t="s">
         <v>62</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="K12" s="34"/>
       <c r="L12" s="33"/>
     </row>
-    <row r="13" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" s="10" customFormat="1">
       <c r="A13" s="47" t="s">
         <v>66</v>
       </c>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="L13" s="33"/>
     </row>
-    <row r="14" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" s="10" customFormat="1">
       <c r="A14" s="42" t="s">
         <v>71</v>
       </c>
@@ -2333,7 +2333,7 @@
       </c>
       <c r="L14" s="33"/>
     </row>
-    <row r="15" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" s="10" customFormat="1">
       <c r="A15" s="42" t="s">
         <v>75</v>
       </c>
@@ -2365,7 +2365,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="10" customFormat="1" ht="105" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" s="10" customFormat="1" ht="105">
       <c r="A16" s="42" t="s">
         <v>79</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="N16" s="35"/>
       <c r="O16" s="35"/>
     </row>
-    <row r="17" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
       <c r="A17" s="43" t="s">
         <v>82</v>
       </c>
@@ -2430,7 +2430,7 @@
       </c>
       <c r="L17" s="33"/>
     </row>
-    <row r="18" spans="1:12" s="34" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" s="34" customFormat="1">
       <c r="A18" s="48" t="s">
         <v>85</v>
       </c>
@@ -2463,7 +2463,7 @@
       </c>
       <c r="L18" s="33"/>
     </row>
-    <row r="19" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" s="10" customFormat="1">
       <c r="A19" s="49" t="s">
         <v>91</v>
       </c>
@@ -2489,9 +2489,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" s="10" customFormat="1" ht="16" customHeight="1">
       <c r="A20" s="50" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>94</v>
@@ -2519,9 +2519,9 @@
       </c>
       <c r="L20" s="33"/>
     </row>
-    <row r="21" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" s="10" customFormat="1">
       <c r="A21" s="51" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B21" s="32" t="s">
         <v>97</v>
@@ -2549,7 +2549,7 @@
       </c>
       <c r="L21" s="33"/>
     </row>
-    <row r="22" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A22" s="42" t="s">
         <v>100</v>
       </c>
@@ -2581,7 +2581,7 @@
       </c>
       <c r="L22" s="33"/>
     </row>
-    <row r="23" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
       <c r="A23" s="42" t="s">
         <v>105</v>
       </c>
@@ -2613,7 +2613,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" s="10" customFormat="1">
       <c r="A24" s="42" t="s">
         <v>109</v>
       </c>
@@ -2645,7 +2645,7 @@
       </c>
       <c r="L24" s="33"/>
     </row>
-    <row r="25" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" s="10" customFormat="1">
       <c r="A25" s="49" t="s">
         <v>113</v>
       </c>
@@ -2677,9 +2677,9 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:12" s="34" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" s="34" customFormat="1" ht="45">
       <c r="A26" s="43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B26" s="32" t="s">
         <v>139</v>
@@ -2688,11 +2688,11 @@
         <v>14</v>
       </c>
       <c r="D26" s="32" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E26" s="33"/>
       <c r="F26" s="30" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J26" s="32" t="s">
         <v>25</v>
@@ -2702,7 +2702,7 @@
       </c>
       <c r="L26" s="33"/>
     </row>
-    <row r="27" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" s="10" customFormat="1">
       <c r="A27" s="50" t="s">
         <v>118</v>
       </c>
@@ -2730,7 +2730,7 @@
       </c>
       <c r="L27" s="12"/>
     </row>
-    <row r="28" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" s="10" customFormat="1">
       <c r="A28" s="42" t="s">
         <v>121</v>
       </c>
@@ -2762,9 +2762,9 @@
       </c>
       <c r="L28" s="33"/>
     </row>
-    <row r="29" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
       <c r="A29" s="43" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B29" s="32" t="s">
         <v>143</v>
@@ -2792,7 +2792,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="30" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" s="10" customFormat="1">
       <c r="A30" s="42" t="s">
         <v>127</v>
       </c>
@@ -2824,12 +2824,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" s="10" customFormat="1">
       <c r="A31" s="53" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B31" s="32" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C31" s="32" t="s">
         <v>14</v>
@@ -2841,7 +2841,7 @@
         <v>34</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
@@ -2853,12 +2853,12 @@
         <v>36</v>
       </c>
       <c r="L31" s="33" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" s="10" customFormat="1">
       <c r="A32" s="43" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B32" s="32" t="s">
         <v>145</v>
@@ -2886,9 +2886,9 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" s="10" customFormat="1">
       <c r="A33" s="42" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B33" s="32" t="s">
         <v>146</v>
@@ -2918,9 +2918,9 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" s="10" customFormat="1">
       <c r="A34" s="42" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B34" s="32" t="s">
         <v>147</v>
@@ -2950,7 +2950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" s="10" customFormat="1">
       <c r="A35" s="42" t="s">
         <v>135</v>
       </c>
@@ -2984,9 +2984,9 @@
       </c>
       <c r="L35" s="33"/>
     </row>
-    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" s="10" customFormat="1">
       <c r="A36" s="42" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B36" s="32" t="s">
         <v>149</v>
@@ -3018,7 +3018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" s="10" customFormat="1">
       <c r="A37" s="52" t="s">
         <v>154</v>
       </c>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="L37" s="33"/>
     </row>
-    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" s="10" customFormat="1">
       <c r="A38" s="42" t="s">
         <v>156</v>
       </c>
@@ -3076,7 +3076,7 @@
       </c>
       <c r="L38" s="33"/>
     </row>
-    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" s="10" customFormat="1">
       <c r="A39" s="42" t="s">
         <v>160</v>
       </c>
@@ -3106,7 +3106,7 @@
       </c>
       <c r="L39" s="33"/>
     </row>
-    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" s="10" customFormat="1">
       <c r="A40" s="49" t="s">
         <v>163</v>
       </c>
@@ -3134,7 +3134,7 @@
       </c>
       <c r="L40" s="12"/>
     </row>
-    <row r="41" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" s="10" customFormat="1">
       <c r="A41" s="53" t="s">
         <v>210</v>
       </c>
@@ -3145,7 +3145,7 @@
         <v>14</v>
       </c>
       <c r="D41" s="32" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E41" s="33" t="s">
         <v>58</v>
@@ -3156,7 +3156,7 @@
       <c r="G41" s="34"/>
       <c r="H41" s="34"/>
       <c r="I41" s="33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J41" s="32" t="s">
         <v>19</v>
@@ -3166,10 +3166,10 @@
       </c>
       <c r="L41" s="33"/>
       <c r="M41" s="10" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" s="10" customFormat="1">
       <c r="A42" s="52" t="s">
         <v>167</v>
       </c>
@@ -3197,7 +3197,7 @@
       </c>
       <c r="L42" s="33"/>
     </row>
-    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" s="10" customFormat="1">
       <c r="A43" s="42" t="s">
         <v>169</v>
       </c>
@@ -3227,7 +3227,7 @@
       </c>
       <c r="L43" s="33"/>
     </row>
-    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" s="10" customFormat="1">
       <c r="A44" s="42" t="s">
         <v>172</v>
       </c>
@@ -3257,7 +3257,7 @@
       </c>
       <c r="L44" s="33"/>
     </row>
-    <row r="45" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" s="10" customFormat="1">
       <c r="A45" s="49" t="s">
         <v>175</v>
       </c>
@@ -3285,21 +3285,21 @@
       </c>
       <c r="L45" s="12"/>
     </row>
-    <row r="46" spans="1:13" s="50" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" s="50" customFormat="1" ht="15">
       <c r="A46" s="54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B46" s="50" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>14</v>
       </c>
       <c r="D46" s="50" t="s">
+        <v>227</v>
+      </c>
+      <c r="F46" s="62" t="s">
         <v>228</v>
-      </c>
-      <c r="F46" s="62" t="s">
-        <v>229</v>
       </c>
       <c r="G46" s="57"/>
       <c r="H46" s="57"/>
@@ -3312,9 +3312,9 @@
       </c>
       <c r="L46" s="58"/>
     </row>
-    <row r="47" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" s="10" customFormat="1">
       <c r="A47" s="53" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="B47" s="32" t="s">
         <v>202</v>
@@ -3323,7 +3323,7 @@
         <v>14</v>
       </c>
       <c r="D47" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E47" s="33" t="s">
         <v>16</v>
@@ -3338,26 +3338,26 @@
         <v>19</v>
       </c>
       <c r="K47" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L47" s="33"/>
     </row>
-    <row r="48" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" s="10" customFormat="1">
       <c r="A48" s="53" t="s">
-        <v>241</v>
+        <v>263</v>
       </c>
       <c r="B48" s="32" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C48" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D48" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E48" s="33"/>
       <c r="F48" s="30" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="G48" s="34"/>
       <c r="H48" s="34"/>
@@ -3366,22 +3366,22 @@
         <v>19</v>
       </c>
       <c r="K48" s="11" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="L48" s="33"/>
     </row>
-    <row r="49" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="51" t="s">
-        <v>238</v>
+    <row r="49" spans="1:12" s="10" customFormat="1">
+      <c r="A49" s="42" t="s">
+        <v>237</v>
       </c>
       <c r="B49" s="32" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C49" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E49" s="33"/>
       <c r="F49" s="30" t="s">
@@ -3400,18 +3400,18 @@
       </c>
       <c r="L49" s="33"/>
     </row>
-    <row r="50" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A50" s="42" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B50" s="32" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C50" s="32" t="s">
         <v>14</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E50" s="33" t="s">
         <v>16</v>
@@ -3432,12 +3432,12 @@
       </c>
       <c r="L50" s="33"/>
     </row>
-    <row r="51" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" s="10" customFormat="1" ht="18" customHeight="1">
       <c r="A51" s="42" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B51" s="32" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C51" s="32" t="s">
         <v>14</v>
@@ -3464,12 +3464,12 @@
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" s="10" customFormat="1">
       <c r="A52" s="42" t="s">
         <v>109</v>
       </c>
       <c r="B52" s="32" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C52" s="32" t="s">
         <v>14</v>
@@ -3496,12 +3496,12 @@
       </c>
       <c r="L52" s="33"/>
     </row>
-    <row r="53" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" s="10" customFormat="1">
       <c r="A53" s="49" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B53" s="32" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C53" s="11" t="s">
         <v>14</v>
@@ -3528,7 +3528,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="1:12" s="10" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" s="10" customFormat="1">
       <c r="A54" s="54" t="s">
         <v>204</v>
       </c>
@@ -3688,13 +3688,13 @@
       <selection activeCell="J20" sqref="J20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
     <col min="2" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" s="2" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3732,7 +3732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" s="2" customFormat="1" ht="68" customHeight="1">
       <c r="A2" s="4" t="s">
         <v>12</v>
       </c>
@@ -3765,7 +3765,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" s="2" customFormat="1">
       <c r="A3" s="4" t="s">
         <v>179</v>
       </c>
@@ -3793,7 +3793,7 @@
       </c>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" s="2" customFormat="1">
       <c r="A4" s="4" t="s">
         <v>180</v>
       </c>
@@ -3842,7 +3842,7 @@
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="33.33203125" style="17" customWidth="1"/>
     <col min="2" max="2" width="30" customWidth="1"/>
@@ -3851,7 +3851,7 @@
     <col min="7" max="241" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="2" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" s="2" customFormat="1">
       <c r="A2" s="25" t="s">
         <v>181</v>
       </c>
@@ -3913,7 +3913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" s="2" customFormat="1">
       <c r="A3" s="24" t="s">
         <v>27</v>
       </c>
@@ -3940,7 +3940,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" s="2" customFormat="1">
       <c r="A4" s="14" t="s">
         <v>31</v>
       </c>
@@ -3969,12 +3969,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" s="2" customFormat="1">
       <c r="A5" s="64" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>14</v>
@@ -3986,7 +3986,7 @@
         <v>34</v>
       </c>
       <c r="F5" s="65" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
@@ -3998,12 +3998,12 @@
         <v>36</v>
       </c>
       <c r="L5" s="21" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1">
       <c r="A6" s="16" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>38</v>
@@ -4028,9 +4028,9 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" s="2" customFormat="1">
       <c r="A7" s="14" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>41</v>
@@ -4057,9 +4057,9 @@
         <v>44</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" s="2" customFormat="1">
       <c r="A8" s="14" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>45</v>
@@ -4086,7 +4086,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A9" s="23" t="s">
         <v>48</v>
       </c>
@@ -4118,7 +4118,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" s="2" customFormat="1" ht="18" customHeight="1">
       <c r="A10" s="23" t="s">
         <v>50</v>
       </c>
@@ -4147,7 +4147,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" s="2" customFormat="1">
       <c r="A11" s="23" t="s">
         <v>56</v>
       </c>
@@ -4179,7 +4179,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" s="2" customFormat="1">
       <c r="A12" s="26" t="s">
         <v>62</v>
       </c>
@@ -4205,7 +4205,7 @@
       <c r="K12" s="20"/>
       <c r="L12" s="21"/>
     </row>
-    <row r="13" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" s="2" customFormat="1">
       <c r="A13" s="15" t="s">
         <v>185</v>
       </c>
@@ -4233,7 +4233,7 @@
       </c>
       <c r="L13" s="21"/>
     </row>
-    <row r="14" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" s="2" customFormat="1">
       <c r="A14" s="22" t="s">
         <v>186</v>
       </c>
@@ -4263,7 +4263,7 @@
       </c>
       <c r="L14" s="21"/>
     </row>
-    <row r="15" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" s="2" customFormat="1">
       <c r="A15" s="22" t="s">
         <v>209</v>
       </c>
@@ -4293,7 +4293,7 @@
       </c>
       <c r="L15" s="21"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" s="2" customFormat="1">
       <c r="A16" s="14" t="s">
         <v>187</v>
       </c>
@@ -4323,7 +4323,7 @@
       <c r="M16" s="4"/>
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" s="2" customFormat="1">
       <c r="A17" s="18" t="s">
         <v>188</v>
       </c>
@@ -4347,7 +4347,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="6"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" s="2" customFormat="1">
       <c r="A18" s="15" t="s">
         <v>190</v>
       </c>
@@ -4375,7 +4375,7 @@
       </c>
       <c r="L18" s="21"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" s="2" customFormat="1">
       <c r="A19" s="22" t="s">
         <v>191</v>
       </c>
@@ -4405,7 +4405,7 @@
       </c>
       <c r="L19" s="21"/>
     </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" s="2" customFormat="1">
       <c r="A20" s="22" t="s">
         <v>192</v>
       </c>
@@ -4435,7 +4435,7 @@
       </c>
       <c r="L20" s="21"/>
     </row>
-    <row r="21" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" s="2" customFormat="1">
       <c r="A21" s="14" t="s">
         <v>194</v>
       </c>
@@ -4465,7 +4465,7 @@
       <c r="M21" s="4"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="1:14" s="4" customFormat="1" ht="14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" s="4" customFormat="1" ht="14">
       <c r="A22" s="14" t="s">
         <v>195</v>
       </c>
@@ -4483,12 +4483,12 @@
         <v>208</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14">
       <c r="A24" s="17" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14">
       <c r="A25" s="29" t="s">
         <v>199</v>
       </c>
@@ -4542,6 +4542,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -4770,27 +4790,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{815FF2A9-0500-4E41-8F16-110FB0128C02}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4809,25 +4828,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A9F8A2F-C3FF-4FEC-AF19-26E26DE76F65}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD20EF80-7752-41E2-9F6E-5CDF83210C62}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>